<commit_message>
feat: made deepseek instead of qwen because of the rate limiter temporarily and added excel file with clusters mapped
</commit_message>
<xml_diff>
--- a/src/llm_judge_evaluation.xlsx
+++ b/src/llm_judge_evaluation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,35 +448,96 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Full Evaluation</t>
+          <t>*   **Coherence</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I will evaluate both reports separately.
-## Report 1: Corporate Restructuring and Regulatory Expansion
-**Coherence:** 9/10
-The report is very coherent. It clearly presents two related developments and consistently links them back to implications for investors. The structure is logical, moving from executive summary to key trends and then actionable insights.
-**Accuracy of Financial Insights:** 8/10
-The financial insights are generally accurate and well-reasoned. The link between proactive restructuring and resilient management is sound, as is the emphasis on broadened due diligence to include cultural and HR practices due to expanded regulatory scope. The anticipation of margin pressure from increased compliance costs is also a valid point.
-**Value to Investors:** 9/10
-This report offers significant value to investors. It highlights emerging risks (conduct risk, regulatory expansion beyond financial metrics) and provides actionable advice (scrutinize governance, broaden due diligence, anticipate sector-wide impact, account for evolving regulatory risk). The discussion of River Island provides a concrete example without getting bogged down in specifics.
-**Clarity of Writing:** 9/10
-The writing is exceptionally clear and concise. The language is professional and accessible, avoiding jargon where possible or explaining it implicitly. The use of bullet points enhances readability, and the executive summary effectively distills the core message.
-***
-## Report 2: Market Volatility and Policy Impact
-**Coherence:** 8/10
-The report is coherent in its overall theme of market volatility and policy impact. Each section flows logically from the executive summary to key trends and then investor implications. All points consistently relate back to the central theme.
-**Accuracy of Financial Insights:** 7/10
-The financial insights are mostly accurate, but some areas could be refined for greater precision or evidence.
-*   **"US service sector growth is stifled as trade wars increase operational costs and lead to job losses."** While trade wars can impact costs and jobs, linking it solely to US service sector *growth being stifled* without further nuance or specific data might be an oversimplification. Service sectors often show different resilience.
-*   **"The rapid decline of Tesla and ascent of BYD in the UK market signals a potent competitive threat..."** While BYD's growth and Tesla's challenges are real, characterising it as a "rapid decline" for Tesla in the *entire UK market* needs more specific data to support the strong claim, especially given the global nature of these companies. It's an important trend but might be stated too definitively.
-*   The overall impact of "investor relief over potential fiscal policy adjustments" on major indices reaching new highs is a reasonable interpretation of market sentiment.
-**Value to Investors:** 8/10
-The report provides good value by alerting investors to current policy-driven impacts and offering strategic advice like focusing on policy-resilient sectors, enhanced due diligence, and a tactical approach to volatility. The warning about the shifting automotive landscape is particularly timely and useful for sector-specific investors.
-**Clarity of Writing:** 9/10
-The writing is clear, direct, and easy to understand. The use of strong topic sentences and bullet points helps to convey complex information efficiently. The language is professional and engaging, making the report accessible to its target audience.
-Here's an illustrative image representing "Market Volatility and Policy Impact":</t>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>*   **Accuracy of Financial Insights</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>*   **Value to Investors</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>*   **Clarity of Writing</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>*   **Coherence</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>*   **Accuracy of Financial Insights</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>*   **Value to Investors</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>*   **Clarity of Writing</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>9</t>
         </is>
       </c>
     </row>

</xml_diff>